<commit_message>
Working on updating the font; the graph itself works.
</commit_message>
<xml_diff>
--- a/BinaryTreeProject-master/TimeDurationComparison.xlsx
+++ b/BinaryTreeProject-master/TimeDurationComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\BinaryTreeProject-master\BinaryTreeProject-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16396B4E-C714-4D7D-A922-CAC35374E885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6642D-DA1B-48EE-B8E3-6F890CF5BADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18180" yWindow="0" windowWidth="17025" windowHeight="10800" xr2:uid="{432D40FB-5E15-486E-A46E-98D79B6ED7BD}"/>
   </bookViews>
@@ -42,28 +42,28 @@
     <t>BinaryTree-Random</t>
   </si>
   <si>
-    <t>Insert 100</t>
-  </si>
-  <si>
-    <t>Insert 10,000</t>
-  </si>
-  <si>
-    <t>Insert 1,000</t>
-  </si>
-  <si>
-    <t>Insert 100,000</t>
-  </si>
-  <si>
-    <t>Delete 100</t>
-  </si>
-  <si>
-    <t>Delete 1,000</t>
-  </si>
-  <si>
-    <t>Delete 10,000</t>
-  </si>
-  <si>
-    <t>Delete 100,000</t>
+    <t>Ins 100</t>
+  </si>
+  <si>
+    <t>Ins 1,000</t>
+  </si>
+  <si>
+    <t>Ins 10,000</t>
+  </si>
+  <si>
+    <t>Ins 100,000</t>
+  </si>
+  <si>
+    <t>Del 100</t>
+  </si>
+  <si>
+    <t>Del 1,000</t>
+  </si>
+  <si>
+    <t>Del 100,000</t>
+  </si>
+  <si>
+    <t>Del 10,000</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1.5630700000000001E-2</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>

<commit_message>
Completed table and plot.
</commit_message>
<xml_diff>
--- a/BinaryTreeProject-master/TimeDurationComparison.xlsx
+++ b/BinaryTreeProject-master/TimeDurationComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\BinaryTreeProject-master\BinaryTreeProject-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6642D-DA1B-48EE-B8E3-6F890CF5BADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF6F142-F723-449C-A857-6482F1AF0A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18180" yWindow="0" windowWidth="17025" windowHeight="10800" xr2:uid="{432D40FB-5E15-486E-A46E-98D79B6ED7BD}"/>
   </bookViews>
@@ -42,28 +42,28 @@
     <t>BinaryTree-Random</t>
   </si>
   <si>
-    <t>Ins 100</t>
-  </si>
-  <si>
-    <t>Ins 1,000</t>
-  </si>
-  <si>
-    <t>Ins 10,000</t>
-  </si>
-  <si>
-    <t>Ins 100,000</t>
-  </si>
-  <si>
-    <t>Del 100</t>
-  </si>
-  <si>
-    <t>Del 1,000</t>
-  </si>
-  <si>
-    <t>Del 100,000</t>
-  </si>
-  <si>
-    <t>Del 10,000</t>
+    <t>I 100</t>
+  </si>
+  <si>
+    <t>I 1,000</t>
+  </si>
+  <si>
+    <t>I 10,000</t>
+  </si>
+  <si>
+    <t>I 100,000</t>
+  </si>
+  <si>
+    <t>D 100</t>
+  </si>
+  <si>
+    <t>D 1,000</t>
+  </si>
+  <si>
+    <t>D 10,000</t>
+  </si>
+  <si>
+    <t>D 100,000</t>
   </si>
 </sst>
 </file>
@@ -99,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +419,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +442,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -455,7 +456,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -526,7 +527,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -540,7 +541,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>